<commit_message>
Adding a front page to the form with project info. Minor corrections.
</commit_message>
<xml_diff>
--- a/AGEO - GeoHazards report.xlsx
+++ b/AGEO - GeoHazards report.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D883FBA-3F4E-449E-8156-DAAB6E772EA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BE0034-84DE-493C-A05A-54AF0E6718DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" tabRatio="542" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1800" yWindow="1965" windowWidth="21600" windowHeight="11385" tabRatio="542" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2154" uniqueCount="1671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2168" uniqueCount="1677">
   <si>
     <t>type</t>
   </si>
@@ -4521,9 +4521,6 @@
     <t>&lt;div width=100% style="background-color: red; text-align: center; vertical-align: top; font-weight: bold; color: white" vertical-align: middle&gt;&lt;img src="sismo.png" /&gt;Sismo&lt;/div&gt;</t>
   </si>
   <si>
-    <t>if(${event_type} != '', '&lt;b&gt;'+jr:choice-name(${event_type}, '${event_type}')+'&lt;/b&gt;', 'Tipo de ocorrência')</t>
-  </si>
-  <si>
     <t>generated_note_calc_title</t>
   </si>
   <si>
@@ -5074,6 +5071,31 @@
   </si>
   <si>
     <t>&lt;p&gt;⚠ Para danos no espaço exterior como:&lt;/p&gt;&lt;br/&gt;&lt;img src="exterior_damages.png" /&gt; &lt;p&gt;&lt;b&gt;Reportar nova ocorrência&lt;/b&gt; através do ecrã principal da aplicação!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>intro</t>
+  </si>
+  <si>
+    <t>logo_CML.png</t>
+  </si>
+  <si>
+    <t>logoAGEO.png</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;
+&lt;font size="0.2" color="dimgrey"&gt;Aplicação disponibilizada por:&lt;/font&gt;
+&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;a href="https://www.lisboa.pt/politica-de-privacidade"&gt;&lt;font size="0.1" color="grey"&gt;Política de privacidade&lt;/font&gt;&lt;/a&gt;&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;
+Aplicação para reporte de eventos relacionados com fenómenos naturais.
+&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>if(${event_type} != '', '&lt;b&gt;'+jr:choice-name(${event_type}, '${event_type}')+'&lt;/b&gt;', '')</t>
   </si>
 </sst>
 </file>
@@ -5218,7 +5240,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5322,12 +5344,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -5681,7 +5707,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tblSurvey" displayName="tblSurvey" ref="A1:AJ159" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tblSurvey" displayName="tblSurvey" ref="A1:AJ165" totalsRowShown="0" headerRowDxfId="20">
   <tableColumns count="36">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="type"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name"/>
@@ -6070,11 +6096,11 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:AJ60"/>
+  <dimension ref="A1:AJ66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6208,7 +6234,7 @@
         <v>1482</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="3" spans="1:36" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -6216,7 +6242,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="C3" s="37" t="s">
         <v>1483</v>
@@ -6225,7 +6251,7 @@
         <v>110</v>
       </c>
       <c r="K3" s="37" t="s">
-        <v>1486</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="4" spans="1:36" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -6233,7 +6259,7 @@
         <v>37</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="C4" s="38" t="s">
         <v>1483</v>
@@ -6242,384 +6268,357 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:36" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+    <row r="5" spans="1:36" s="45" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:36" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="45" t="s">
+        <v>1670</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>1489</v>
+      </c>
+      <c r="F6" s="45" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>1489</v>
+      </c>
+      <c r="R7" s="45" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" s="45" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" s="45" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>1673</v>
+      </c>
+      <c r="D9" s="45" t="s">
+        <v>1674</v>
+      </c>
+      <c r="R9" s="45" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="32" t="s">
         <v>1464</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C12" s="32" t="s">
         <v>1465</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F12" s="32" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>1489</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="R13" s="32" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:35" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>1479</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>1484</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="N17" s="37" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>1485</v>
+      </c>
+      <c r="N18" s="37" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>1481</v>
+      </c>
+      <c r="AH19" s="37" t="s">
+        <v>1523</v>
+      </c>
+      <c r="AI19" s="37" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="39" t="s">
         <v>1492</v>
       </c>
-      <c r="B7" s="32" t="s">
-        <v>1466</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>1490</v>
-      </c>
-      <c r="F7" s="32" t="s">
+      <c r="C20" s="39" t="s">
+        <v>1493</v>
+      </c>
+      <c r="J20" s="39" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="39" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>1496</v>
+      </c>
+      <c r="C21" s="39" t="s">
+        <v>1489</v>
+      </c>
+      <c r="T21" s="39" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="39" t="s">
+        <v>1512</v>
+      </c>
+      <c r="B22" s="39" t="s">
+        <v>1511</v>
+      </c>
+      <c r="C22" s="39" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="37" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A25" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>1520</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>1489</v>
+      </c>
+      <c r="F25" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="N25" s="32" t="s">
+        <v>1521</v>
+      </c>
+      <c r="P25" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="40" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>1528</v>
+      </c>
+      <c r="F26" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="R7" s="32" t="s">
-        <v>1531</v>
-      </c>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:36" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:36" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
-        <v>100</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>1479</v>
-      </c>
-      <c r="C11" s="37" t="s">
-        <v>1484</v>
-      </c>
-      <c r="F11" s="37" t="s">
-        <v>181</v>
-      </c>
-      <c r="N11" s="37" t="s">
-        <v>1499</v>
-      </c>
-    </row>
-    <row r="12" spans="1:36" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="37" t="s">
-        <v>1485</v>
-      </c>
-      <c r="N12" s="37" t="s">
-        <v>1532</v>
-      </c>
-    </row>
-    <row r="13" spans="1:36" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="37" t="s">
-        <v>1480</v>
-      </c>
-      <c r="C13" s="37" t="s">
-        <v>1481</v>
-      </c>
-      <c r="AH13" s="37" t="s">
-        <v>1524</v>
-      </c>
-      <c r="AI13" s="37" t="s">
-        <v>1525</v>
-      </c>
-    </row>
-    <row r="14" spans="1:36" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="39" t="s">
-        <v>1493</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>1494</v>
-      </c>
-      <c r="J14" s="39" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="15" spans="1:36" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
-        <v>1498</v>
-      </c>
-      <c r="B15" s="39" t="s">
-        <v>1497</v>
-      </c>
-      <c r="C15" s="39" t="s">
-        <v>1490</v>
-      </c>
-      <c r="T15" s="39" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="16" spans="1:36" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
-        <v>1513</v>
-      </c>
-      <c r="B16" s="39" t="s">
-        <v>1512</v>
-      </c>
-      <c r="C16" s="39" t="s">
-        <v>1514</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="B19" s="32" t="s">
-        <v>1521</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>1490</v>
-      </c>
-      <c r="F19" s="32" t="s">
-        <v>181</v>
-      </c>
-      <c r="N19" s="32" t="s">
-        <v>1522</v>
-      </c>
-      <c r="P19" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="40" t="s">
-        <v>1528</v>
-      </c>
-      <c r="B20" s="40" t="s">
-        <v>1526</v>
-      </c>
-      <c r="C20" s="40" t="s">
+      <c r="R26" s="40" t="s">
         <v>1529</v>
       </c>
-      <c r="F20" s="40" t="s">
+    </row>
+    <row r="27" spans="1:35" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="40" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>1538</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>1539</v>
+      </c>
+      <c r="F27" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="R20" s="40" t="s">
-        <v>1530</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
-        <v>1538</v>
-      </c>
-      <c r="B21" s="40" t="s">
-        <v>1539</v>
-      </c>
-      <c r="C21" s="40" t="s">
+      <c r="R27" s="40" t="s">
         <v>1540</v>
       </c>
-      <c r="F21" s="40" t="s">
+    </row>
+    <row r="28" spans="1:35" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="41" t="s">
+        <v>1555</v>
+      </c>
+      <c r="B28" s="41" t="s">
+        <v>1541</v>
+      </c>
+      <c r="C28" s="41" t="s">
+        <v>1542</v>
+      </c>
+      <c r="F28" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="R21" s="40" t="s">
-        <v>1541</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="41" t="s">
+      <c r="R28" s="41" t="s">
         <v>1556</v>
       </c>
-      <c r="B22" s="41" t="s">
-        <v>1542</v>
-      </c>
-      <c r="C22" s="41" t="s">
-        <v>1543</v>
-      </c>
-      <c r="F22" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="R22" s="41" t="s">
+    </row>
+    <row r="29" spans="1:35" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="42" t="s">
+        <v>1559</v>
+      </c>
+      <c r="B29" s="42" t="s">
         <v>1557</v>
       </c>
-    </row>
-    <row r="23" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="42" t="s">
-        <v>1560</v>
-      </c>
-      <c r="B23" s="42" t="s">
+      <c r="C29" s="42" t="s">
         <v>1558</v>
       </c>
-      <c r="C23" s="42" t="s">
-        <v>1559</v>
-      </c>
-      <c r="F23" s="42" t="s">
+      <c r="F29" s="42" t="s">
         <v>141</v>
-      </c>
-      <c r="T23" s="42" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="B26" s="42" t="s">
-        <v>1567</v>
-      </c>
-      <c r="C26" s="42" t="s">
-        <v>1490</v>
-      </c>
-      <c r="F26" s="42" t="s">
-        <v>181</v>
-      </c>
-      <c r="N26" s="42" t="s">
-        <v>1587</v>
-      </c>
-      <c r="P26" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="42" t="s">
-        <v>1588</v>
-      </c>
-      <c r="B27" s="42" t="s">
-        <v>1568</v>
-      </c>
-      <c r="C27" s="42" t="s">
-        <v>1569</v>
-      </c>
-      <c r="F27" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="R27" s="42" t="s">
-        <v>1586</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="42" t="s">
-        <v>1570</v>
-      </c>
-      <c r="C28" s="42" t="s">
-        <v>1571</v>
-      </c>
-      <c r="F28" s="42" t="s">
-        <v>143</v>
-      </c>
-      <c r="N28" s="42" t="s">
-        <v>1573</v>
-      </c>
-      <c r="W28" s="42" t="s">
-        <v>1572</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="42" t="s">
-        <v>1592</v>
-      </c>
-      <c r="B29" s="42" t="s">
-        <v>1590</v>
-      </c>
-      <c r="C29" s="42" t="s">
-        <v>1591</v>
-      </c>
-      <c r="F29" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="R29" s="42" t="s">
-        <v>1599</v>
       </c>
       <c r="T29" s="42" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="30" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="42" t="s">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A30" s="32" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" s="42" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:35" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="42" t="s">
         <v>104</v>
       </c>
       <c r="B32" s="42" t="s">
-        <v>1600</v>
+        <v>1566</v>
       </c>
       <c r="C32" s="42" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="F32" s="42" t="s">
         <v>181</v>
       </c>
       <c r="N32" s="42" t="s">
-        <v>1613</v>
+        <v>1586</v>
       </c>
       <c r="P32" s="42">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="43" t="s">
-        <v>1604</v>
-      </c>
-      <c r="B33" s="43" t="s">
-        <v>1601</v>
-      </c>
-      <c r="C33" s="43" t="s">
+    <row r="33" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="42" t="s">
+        <v>1587</v>
+      </c>
+      <c r="B33" s="42" t="s">
+        <v>1567</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>1568</v>
+      </c>
+      <c r="F33" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="R33" s="42" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="42" t="s">
         <v>1569</v>
       </c>
-      <c r="F33" s="43" t="s">
+      <c r="C34" s="42" t="s">
+        <v>1570</v>
+      </c>
+      <c r="F34" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="N34" s="42" t="s">
+        <v>1572</v>
+      </c>
+      <c r="W34" s="42" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="42" t="s">
+        <v>1591</v>
+      </c>
+      <c r="B35" s="42" t="s">
+        <v>1589</v>
+      </c>
+      <c r="C35" s="42" t="s">
+        <v>1590</v>
+      </c>
+      <c r="F35" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="R33" s="43" t="s">
-        <v>1608</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" s="43" t="s">
-        <v>1602</v>
-      </c>
-      <c r="C34" s="43" t="s">
-        <v>1571</v>
-      </c>
-      <c r="F34" s="43" t="s">
-        <v>143</v>
-      </c>
-      <c r="N34" s="43" t="s">
-        <v>1603</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="43" t="s">
-        <v>1612</v>
-      </c>
-      <c r="B35" s="43" t="s">
-        <v>1609</v>
-      </c>
-      <c r="C35" s="43" t="s">
-        <v>1610</v>
-      </c>
-      <c r="F35" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="R35" s="43" t="s">
-        <v>1611</v>
-      </c>
-      <c r="T35" s="43" t="s">
+      <c r="R35" s="42" t="s">
+        <v>1598</v>
+      </c>
+      <c r="T35" s="42" t="s">
         <v>205</v>
       </c>
     </row>
@@ -6628,304 +6627,384 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="44" t="s">
+    <row r="37" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="B38" s="44" t="s">
-        <v>1614</v>
-      </c>
-      <c r="C38" s="44" t="s">
-        <v>1490</v>
-      </c>
-      <c r="F38" s="44" t="s">
+      <c r="B38" s="42" t="s">
+        <v>1599</v>
+      </c>
+      <c r="C38" s="42" t="s">
+        <v>1489</v>
+      </c>
+      <c r="F38" s="42" t="s">
         <v>181</v>
       </c>
-      <c r="N38" s="44" t="s">
-        <v>1615</v>
-      </c>
-      <c r="P38" s="44">
+      <c r="N38" s="42" t="s">
+        <v>1612</v>
+      </c>
+      <c r="P38" s="42">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="44" t="s">
-        <v>1617</v>
-      </c>
-      <c r="B39" s="44" t="s">
-        <v>1616</v>
-      </c>
-      <c r="C39" s="44" t="s">
-        <v>1620</v>
-      </c>
-      <c r="F39" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="T39" s="44" t="s">
+    <row r="39" spans="1:23" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="43" t="s">
+        <v>1603</v>
+      </c>
+      <c r="B39" s="43" t="s">
+        <v>1600</v>
+      </c>
+      <c r="C39" s="43" t="s">
+        <v>1568</v>
+      </c>
+      <c r="F39" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="R39" s="43" t="s">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="43" t="s">
+        <v>1601</v>
+      </c>
+      <c r="C40" s="43" t="s">
+        <v>1570</v>
+      </c>
+      <c r="F40" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="N40" s="43" t="s">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="43" t="s">
+        <v>1611</v>
+      </c>
+      <c r="B41" s="43" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C41" s="43" t="s">
+        <v>1609</v>
+      </c>
+      <c r="F41" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="R41" s="43" t="s">
+        <v>1610</v>
+      </c>
+      <c r="T41" s="43" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="40" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="44" t="s">
-        <v>1623</v>
-      </c>
-      <c r="B40" s="44" t="s">
-        <v>1621</v>
-      </c>
-      <c r="C40" s="44" t="s">
-        <v>1622</v>
-      </c>
-      <c r="F40" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="R40" s="44" t="s">
-        <v>1627</v>
-      </c>
-    </row>
-    <row r="41" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="B41" s="44" t="s">
-        <v>1625</v>
-      </c>
-      <c r="C41" s="44" t="s">
-        <v>1626</v>
-      </c>
-      <c r="F41" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="N41" s="44" t="s">
-        <v>1624</v>
-      </c>
-    </row>
-    <row r="42" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="44" t="s">
-        <v>1634</v>
-      </c>
-      <c r="B42" s="44" t="s">
-        <v>1636</v>
-      </c>
-      <c r="C42" s="44" t="s">
-        <v>1632</v>
-      </c>
-      <c r="F42" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="R42" s="44" t="s">
-        <v>1633</v>
-      </c>
-    </row>
-    <row r="43" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="B43" s="44" t="s">
-        <v>1637</v>
-      </c>
-      <c r="C43" s="44" t="s">
-        <v>1585</v>
-      </c>
-      <c r="F43" s="44" t="s">
-        <v>143</v>
-      </c>
-      <c r="N43" s="44" t="s">
-        <v>1635</v>
-      </c>
-      <c r="W43" s="44" t="s">
-        <v>1572</v>
+    <row r="42" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="42" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="44" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>104</v>
+      </c>
+      <c r="B44" s="44" t="s">
+        <v>1613</v>
+      </c>
+      <c r="C44" s="44" t="s">
+        <v>1489</v>
+      </c>
+      <c r="F44" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="N44" s="44" t="s">
+        <v>1614</v>
+      </c>
+      <c r="P44" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="44" t="s">
+        <v>1616</v>
+      </c>
+      <c r="B45" s="44" t="s">
+        <v>1615</v>
+      </c>
+      <c r="C45" s="44" t="s">
+        <v>1619</v>
+      </c>
+      <c r="F45" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="T45" s="44" t="s">
+        <v>205</v>
+      </c>
+    </row>
     <row r="46" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="44" t="s">
-        <v>104</v>
+        <v>1622</v>
       </c>
       <c r="B46" s="44" t="s">
-        <v>1651</v>
+        <v>1620</v>
       </c>
       <c r="C46" s="44" t="s">
-        <v>1655</v>
+        <v>1621</v>
       </c>
       <c r="F46" s="44" t="s">
-        <v>181</v>
-      </c>
-      <c r="N46" s="44" t="s">
-        <v>1650</v>
+        <v>36</v>
+      </c>
+      <c r="R46" s="44" t="s">
+        <v>1626</v>
       </c>
     </row>
     <row r="47" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="44" t="s">
-        <v>1654</v>
+        <v>63</v>
       </c>
       <c r="B47" s="44" t="s">
-        <v>1656</v>
+        <v>1624</v>
       </c>
       <c r="C47" s="44" t="s">
-        <v>1490</v>
+        <v>1625</v>
       </c>
       <c r="F47" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="R47" s="44" t="s">
-        <v>1666</v>
+        <v>148</v>
+      </c>
+      <c r="N47" s="44" t="s">
+        <v>1623</v>
       </c>
     </row>
     <row r="48" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="44" t="s">
-        <v>66</v>
+        <v>1633</v>
       </c>
       <c r="B48" s="44" t="s">
-        <v>1652</v>
+        <v>1635</v>
       </c>
       <c r="C48" s="44" t="s">
-        <v>1653</v>
+        <v>1631</v>
       </c>
       <c r="F48" s="44" t="s">
-        <v>158</v>
-      </c>
-      <c r="J48" s="44">
-        <v>1</v>
-      </c>
-      <c r="T48" s="44" t="s">
-        <v>205</v>
+        <v>36</v>
+      </c>
+      <c r="R48" s="44" t="s">
+        <v>1632</v>
       </c>
     </row>
     <row r="49" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" s="44" t="s">
+        <v>1636</v>
+      </c>
+      <c r="C49" s="44" t="s">
+        <v>1584</v>
+      </c>
+      <c r="F49" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="N49" s="44" t="s">
+        <v>1634</v>
+      </c>
+      <c r="W49" s="44" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="44" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:23" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A51" s="32" t="s">
+    <row r="51" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="B52" s="44" t="s">
+        <v>1650</v>
+      </c>
+      <c r="C52" s="44" t="s">
+        <v>1654</v>
+      </c>
+      <c r="F52" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="N52" s="44" t="s">
+        <v>1649</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="44" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B53" s="44" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C53" s="44" t="s">
+        <v>1489</v>
+      </c>
+      <c r="F53" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="R53" s="44" t="s">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="44" t="s">
+        <v>1651</v>
+      </c>
+      <c r="C54" s="44" t="s">
+        <v>1652</v>
+      </c>
+      <c r="F54" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="J54" s="44">
+        <v>1</v>
+      </c>
+      <c r="T54" s="44" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A57" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="B51" s="32" t="s">
+      <c r="B57" s="32" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C57" s="32" t="s">
+        <v>1517</v>
+      </c>
+      <c r="F57" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="N57" s="39" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" s="39" t="s">
+        <v>1518</v>
+      </c>
+      <c r="C58" s="39" t="s">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B59" s="39" t="s">
         <v>1516</v>
       </c>
-      <c r="C51" s="32" t="s">
-        <v>1518</v>
-      </c>
-      <c r="F51" s="32" t="s">
+      <c r="C59" s="39" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" s="39" t="s">
+        <v>1467</v>
+      </c>
+      <c r="C61" s="39" t="s">
+        <v>1468</v>
+      </c>
+      <c r="F61" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="W61" s="39" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A62" s="32" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="B64" s="44" t="s">
+        <v>1648</v>
+      </c>
+      <c r="C64" s="44" t="s">
+        <v>1489</v>
+      </c>
+      <c r="F64" s="44" t="s">
         <v>181</v>
       </c>
-      <c r="N51" s="39" t="s">
-        <v>1499</v>
-      </c>
-    </row>
-    <row r="52" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="B52" s="39" t="s">
-        <v>1519</v>
-      </c>
-      <c r="C52" s="39" t="s">
-        <v>1490</v>
-      </c>
-    </row>
-    <row r="53" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="B53" s="39" t="s">
-        <v>1517</v>
-      </c>
-      <c r="C53" s="39" t="s">
-        <v>1518</v>
-      </c>
-    </row>
-    <row r="54" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="39" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="B55" s="39" t="s">
-        <v>1467</v>
-      </c>
-      <c r="C55" s="39" t="s">
-        <v>1468</v>
-      </c>
-      <c r="F55" s="39" t="s">
-        <v>143</v>
-      </c>
-      <c r="W55" s="39" t="s">
-        <v>1520</v>
-      </c>
-    </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A56" s="32" t="s">
+      <c r="N64" s="44" t="s">
+        <v>1649</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="C65" s="44" t="s">
+        <v>1669</v>
+      </c>
+      <c r="W65" s="44" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="44" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="B58" s="44" t="s">
-        <v>1649</v>
-      </c>
-      <c r="C58" s="44" t="s">
-        <v>1490</v>
-      </c>
-      <c r="F58" s="44" t="s">
-        <v>181</v>
-      </c>
-      <c r="N58" s="44" t="s">
-        <v>1650</v>
-      </c>
-    </row>
-    <row r="59" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="C59" s="44" t="s">
-        <v>1670</v>
-      </c>
-      <c r="W59" s="44" t="s">
-        <v>1669</v>
-      </c>
-    </row>
-    <row r="60" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="44" t="s">
-        <v>102</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B159">
-    <cfRule type="duplicateValues" dxfId="0" priority="13"/>
+  <conditionalFormatting sqref="B2:B165">
+    <cfRule type="duplicateValues" dxfId="0" priority="14"/>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" sqref="A2:A159" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="A2:A165" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>QuestionTypes</formula1>
     </dataValidation>
-    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Name" error="Names must be unique and cannot contain spaces, non-ASCII characters, reserved keywords, or special symbols. For ArcGIS Enterprise feature layers, names must not exceed 31 characters." sqref="B2:B159" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Name" error="Names must be unique and cannot contain spaces, non-ASCII characters, reserved keywords, or special symbols. For ArcGIS Enterprise feature layers, names must not exceed 31 characters." sqref="B2:B165" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>AND(LEN(B2)=LEN(SUBSTITUTE(B2," ","")),LEN(B2)&lt;32,COUNTIF(Reserved,B2) = 0,SUMPRODUCT(--ISNUMBER(SEARCH(SpecialChars,B2)))=0)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="I2:I159 G2:G159" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" sqref="G2:G165 I2:I165" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Bind Type" error="The value you have entered is not one of the supported bind types." sqref="S2:S159" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Bind Type" error="The value you have entered is not one of the supported bind types." sqref="S2:S165" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>BindTypes</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Field Type" error="The value you have entered is not one of the supported field types." sqref="T2:T159" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Field Type" error="The value you have entered is not one of the supported field types." sqref="T2:T165" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>EsriFieldTypes</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Field Length" error="Please enter a whole number greater than zero." sqref="U2:U159" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Field Length" error="Please enter a whole number greater than zero." sqref="U2:U165" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F159" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F165" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>IF(LEFT(A2,4)="rank",appearRank,IF(LEFT(A2,8)="select_m",appearSelMulti,IF(LEFT(A2,8)="select_o",appearSelOne,IF(A2="begin group",appearBeginGrp,IF(A2="begin repeat",appearBeginRpt,INDIRECT("appear"&amp;A2))))))</formula1>
     </dataValidation>
   </dataValidations>
@@ -6988,7 +7067,7 @@
         <v>52</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -6999,7 +7078,7 @@
         <v>1472</v>
       </c>
       <c r="C4" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -7009,10 +7088,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="B6" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="C6" t="s">
         <v>1473</v>
@@ -7020,10 +7099,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="B7" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="C7" t="s">
         <v>1474</v>
@@ -7031,10 +7110,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="B8" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="C8" t="s">
         <v>1475</v>
@@ -7042,10 +7121,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="B9" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="C9" t="s">
         <v>1476</v>
@@ -7053,10 +7132,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="39" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="B10" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="C10" t="s">
         <v>1477</v>
@@ -7064,10 +7143,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="39" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="B11" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="C11" t="s">
         <v>1478</v>
@@ -7080,13 +7159,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -7096,35 +7175,35 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B15" t="s">
         <v>1505</v>
       </c>
-      <c r="B15" t="s">
-        <v>1506</v>
-      </c>
       <c r="C15" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="39" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="B16" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="C16" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="39" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="B17" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="C17" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -7134,7 +7213,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -7145,7 +7224,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="40" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -7156,7 +7235,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -7167,7 +7246,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -7178,24 +7257,24 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B24" t="s">
         <v>1533</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>1534</v>
-      </c>
-      <c r="C24" t="s">
-        <v>1535</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="B25" t="s">
+        <v>1535</v>
+      </c>
+      <c r="C25" t="s">
         <v>1536</v>
-      </c>
-      <c r="C25" t="s">
-        <v>1537</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -7205,68 +7284,68 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>1543</v>
+      </c>
+      <c r="B27" t="s">
         <v>1544</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>1545</v>
-      </c>
-      <c r="C27" t="s">
-        <v>1546</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="B28" t="s">
         <v>132</v>
       </c>
       <c r="C28" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="41" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="B29" t="s">
+        <v>1547</v>
+      </c>
+      <c r="C29" t="s">
         <v>1548</v>
-      </c>
-      <c r="C29" t="s">
-        <v>1549</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="41" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="B30" t="s">
+        <v>1549</v>
+      </c>
+      <c r="C30" t="s">
         <v>1550</v>
-      </c>
-      <c r="C30" t="s">
-        <v>1551</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="41" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="B31" t="s">
+        <v>1551</v>
+      </c>
+      <c r="C31" t="s">
         <v>1552</v>
-      </c>
-      <c r="C31" t="s">
-        <v>1553</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="B32" t="s">
+        <v>1553</v>
+      </c>
+      <c r="C32" t="s">
         <v>1554</v>
-      </c>
-      <c r="C32" t="s">
-        <v>1555</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -7276,57 +7355,57 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="42" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="B35">
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="B36">
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="42" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="B37">
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="42" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="B38">
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -7336,68 +7415,68 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="B40" s="32" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="42" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="B41" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="C41" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="42" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="B42" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="C42" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="42" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="B43" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="C43" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="42" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="B44" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="C44" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="42" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="B45" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="C45" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -7407,57 +7486,57 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="42" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="B48">
         <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="42" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="B49">
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="42" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="B50" s="32">
         <v>4</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="42" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="B51">
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -7467,68 +7546,68 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="B53" s="43" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="C53" s="43" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="43" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="B54" s="43" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="C54" s="43" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="43" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="B55" s="43" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="C55" s="43" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="43" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="B56" s="43" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="C56" s="43" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="43" t="s">
+        <v>1604</v>
+      </c>
+      <c r="B57" s="43" t="s">
+        <v>1606</v>
+      </c>
+      <c r="C57" s="43" t="s">
         <v>1605</v>
-      </c>
-      <c r="B57" s="43" t="s">
-        <v>1607</v>
-      </c>
-      <c r="C57" s="43" t="s">
-        <v>1606</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="43" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="B58" s="43" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="C58" s="43" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -7538,7 +7617,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -7549,7 +7628,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="43" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -7560,7 +7639,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="43" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="B62">
         <v>3</v>
@@ -7571,7 +7650,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="43" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="B63" s="32">
         <v>4</v>
@@ -7582,7 +7661,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="43" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="B64">
         <v>5</v>
@@ -7593,7 +7672,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="43" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="B65">
         <v>6</v>
@@ -7609,7 +7688,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -7620,7 +7699,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="44" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -7631,7 +7710,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="44" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="B69">
         <v>3</v>
@@ -7642,7 +7721,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="44" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="B70">
         <v>4</v>
@@ -7653,7 +7732,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="44" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="B71">
         <v>5</v>
@@ -7664,13 +7743,13 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="44" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="B72">
         <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -7680,46 +7759,46 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="B74" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="C74" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="44" t="s">
+        <v>1627</v>
+      </c>
+      <c r="B75" t="s">
         <v>1628</v>
       </c>
-      <c r="B75" t="s">
-        <v>1629</v>
-      </c>
       <c r="C75" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="44" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="B76" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="C76" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="44" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="B77" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="C77" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -7729,68 +7808,68 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="44" t="s">
+        <v>1637</v>
+      </c>
+      <c r="B79" t="s">
         <v>1638</v>
       </c>
-      <c r="B79" t="s">
-        <v>1639</v>
-      </c>
       <c r="C79" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="44" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="B80" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="C80" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="44" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="B81" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="C81" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="44" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="B82" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="C82" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="44" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="B83" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="C83" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="44" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="B84" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="C84" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -7800,46 +7879,46 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>1656</v>
+      </c>
+      <c r="B86" t="s">
         <v>1657</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
         <v>1658</v>
-      </c>
-      <c r="C86" t="s">
-        <v>1659</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="44" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="B87" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="C87" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="44" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="B88" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="C88" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="44" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="B89" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="C89" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -8546,7 +8625,7 @@
         <v>1469</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="G2" s="32" t="s">
         <v>1470</v>
@@ -8587,10 +8666,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="46"/>
+      <c r="B1" s="47"/>
       <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8615,10 +8694,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="46"/>
+      <c r="B6" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Actualizações de logos e de image-maps.
</commit_message>
<xml_diff>
--- a/AGEO - GeoHazards report.xlsx
+++ b/AGEO - GeoHazards report.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A8031F-D890-4DD2-8BB5-D0FF1F4E91BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E3DD66-DFEE-4CED-A8F5-7798C1CE9027}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1965" windowWidth="21600" windowHeight="11385" tabRatio="542" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6225" yWindow="3855" windowWidth="21600" windowHeight="11385" tabRatio="542" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2170" uniqueCount="1678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2227" uniqueCount="1697">
   <si>
     <t>type</t>
   </si>
@@ -4458,9 +4458,6 @@
     <t>geohazard_type</t>
   </si>
   <si>
-    <t>Selecione o tipo de ocorrência</t>
-  </si>
-  <si>
     <t>event_type</t>
   </si>
   <si>
@@ -4506,18 +4503,12 @@
     <t>event_point</t>
   </si>
   <si>
-    <t>&lt;b&gt;Localização&lt;/b&gt;</t>
-  </si>
-  <si>
     <t>generated_note_form_title</t>
   </si>
   <si>
     <t>no label</t>
   </si>
   <si>
-    <t>Informação sobre o evento</t>
-  </si>
-  <si>
     <t>generated_note_calc_title</t>
   </si>
   <si>
@@ -4539,9 +4530,6 @@
     <t>event_date</t>
   </si>
   <si>
-    <t>Data do evento</t>
-  </si>
-  <si>
     <t>live_event</t>
   </si>
   <si>
@@ -4599,24 +4587,15 @@
     <t>select_multiple elements_at_risk_list</t>
   </si>
   <si>
-    <t>Elementos em risco</t>
-  </si>
-  <si>
     <t>landslide</t>
   </si>
   <si>
     <t>photos_page</t>
   </si>
   <si>
-    <t>foto</t>
-  </si>
-  <si>
     <t>Fotos</t>
   </si>
   <si>
-    <t>photos</t>
-  </si>
-  <si>
     <t>defaultHeight=6</t>
   </si>
   <si>
@@ -4644,9 +4623,6 @@
     <t>select_one building_settlement_list</t>
   </si>
   <si>
-    <t>Tipo de assentamento</t>
-  </si>
-  <si>
     <t>building_settlement.svg</t>
   </si>
   <si>
@@ -4674,18 +4650,12 @@
     <t>other_structures</t>
   </si>
   <si>
-    <t>Outras estruturas</t>
-  </si>
-  <si>
     <t>settlement_other_structures.svg</t>
   </si>
   <si>
     <t>crack_direction</t>
   </si>
   <si>
-    <t>Direcção da fissuração</t>
-  </si>
-  <si>
     <t>crack_direction_list</t>
   </si>
   <si>
@@ -4731,9 +4701,6 @@
     <t>crack_dim</t>
   </si>
   <si>
-    <t>Dimensão das fissuras</t>
-  </si>
-  <si>
     <t>select_one crack_dim_list</t>
   </si>
   <si>
@@ -4761,9 +4728,6 @@
     <t>damages</t>
   </si>
   <si>
-    <t>Danos observados</t>
-  </si>
-  <si>
     <t>damages_other</t>
   </si>
   <si>
@@ -4827,9 +4791,6 @@
     <t>volume</t>
   </si>
   <si>
-    <t>Volume de terras deslocadas</t>
-  </si>
-  <si>
     <t>select_one volume_list</t>
   </si>
   <si>
@@ -4884,9 +4845,6 @@
     <t>water_level</t>
   </si>
   <si>
-    <t>Nível de água</t>
-  </si>
-  <si>
     <t>water_level.svg</t>
   </si>
   <si>
@@ -4914,15 +4872,9 @@
     <t>≥ 6</t>
   </si>
   <si>
-    <t>&lt;p&gt;Dimensão (em passos)&lt;p/&gt;&lt;img src="steps.png" /&gt;</t>
-  </si>
-  <si>
     <t>sinkhole_location</t>
   </si>
   <si>
-    <t>Local</t>
-  </si>
-  <si>
     <t>select_one sinkhole_location_list</t>
   </si>
   <si>
@@ -4950,9 +4902,6 @@
     <t>Zona pedonal</t>
   </si>
   <si>
-    <t>Infraestruturas afetadas</t>
-  </si>
-  <si>
     <t>urban_infrastructures.svg</t>
   </si>
   <si>
@@ -5019,9 +4968,6 @@
     <t>select_one building_damages_list</t>
   </si>
   <si>
-    <t>Danos em edifícios</t>
-  </si>
-  <si>
     <t>damage_level</t>
   </si>
   <si>
@@ -5064,9 +5010,6 @@
     <t>border=2</t>
   </si>
   <si>
-    <t>&lt;p&gt;⚠ Para danos no espaço exterior como:&lt;/p&gt;&lt;br/&gt;&lt;img src="exterior_damages.png" /&gt; &lt;p&gt;&lt;b&gt;Reportar nova ocorrência&lt;/b&gt; através do ecrã principal da aplicação!&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>intro</t>
   </si>
   <si>
@@ -5076,29 +5019,143 @@
     <t>logoAGEO.png</t>
   </si>
   <si>
+    <t>&lt;center&gt;&lt;a href="https://www.lisboa.pt/politica-de-privacidade"&gt;&lt;font size="0.1" color="grey"&gt;Política de privacidade&lt;/font&gt;&lt;/a&gt;&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>if(${event_type} != '', '&lt;b&gt;'+jr:choice-name(${event_type}, '${event_type}')+'&lt;/b&gt;', '')</t>
+  </si>
+  <si>
+    <t>tsunami</t>
+  </si>
+  <si>
+    <t>Tsunami</t>
+  </si>
+  <si>
+    <t>Interreg+cloud.png</t>
+  </si>
+  <si>
+    <t>query</t>
+  </si>
+  <si>
+    <t>Indique a localização da ocorrência</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;font size="3" style="font-family: Calibri, fantasy; font-weight: bold"&gt;
+Aplicação para reporte de eventos relacionados com fenómenos naturais.
+&lt;/font&gt;&lt;/center&gt;</t>
+  </si>
+  <si>
     <t>&lt;center&gt;
-&lt;font size="0.2" color="dimgrey"&gt;Aplicação disponibilizada por:&lt;/font&gt;
+&lt;font size="0.1" color="dimgrey" style="font-family: Calibri, fantasy"&gt;Aplicação disponibilizada por:&lt;/font&gt;
 &lt;/center&gt;</t>
   </si>
   <si>
-    <t>&lt;center&gt;&lt;a href="https://www.lisboa.pt/politica-de-privacidade"&gt;&lt;font size="0.1" color="grey"&gt;Política de privacidade&lt;/font&gt;&lt;/a&gt;&lt;/center&gt;</t>
-  </si>
-  <si>
-    <t>&lt;center&gt;
-Aplicação para reporte de eventos relacionados com fenómenos naturais.
-&lt;/center&gt;</t>
-  </si>
-  <si>
-    <t>if(${event_type} != '', '&lt;b&gt;'+jr:choice-name(${event_type}, '${event_type}')+'&lt;/b&gt;', '')</t>
-  </si>
-  <si>
-    <t>&lt;i&gt;(Volume equivalente a)&lt;/i&gt;</t>
-  </si>
-  <si>
-    <t>tsunami</t>
-  </si>
-  <si>
-    <t>Tsunami</t>
+    <t>rochas.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="line-height: 50px"&gt; &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Riska_lupa.png</t>
+  </si>
+  <si>
+    <t>exterior_damages.png</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;font size="3" style="font-family: Calibri, fantasy"&gt;&lt;p&gt;⚠ Para danos no espaço exterior como:&lt;/p&gt;&lt;/font&gt;&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;font size="3" style="font-family: Calibri, fantasy"&gt;&lt;br/&gt;&lt;b&gt;Reportar nova ocorrência&lt;/b&gt; através do ecrã principal da aplicação!&lt;/font&gt;&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;Selecione o tipo de ocorrência&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;Informação sobre o evento&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;Localização&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>&lt;br/&gt;&lt;center&gt;Elementos em risco&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>&lt;br/&gt;&lt;center&gt;Data do evento&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;b&gt;Danos observados&lt;/center&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;b&gt;Volume de terras deslocadas&lt;/center&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;i&gt;(Volume equivalente a)&lt;/i&gt;&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;b&gt;Tipo de assentamento&lt;/b&gt;&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;b&gt;Outras estruturas&lt;/b&gt;&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;b&gt;Direcção da fissuração&lt;/b&gt;&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;b&gt;Dimensão das fissuras&lt;/b&gt;&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;b&gt;Nível de água&lt;/center&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;b&gt;Dimensão (em passos)&lt;/center&gt;&lt;/b&gt;&lt;br/&gt;&lt;img src="steps.png" /&gt;</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;b&gt;Infraestruturas afetadas&lt;/center&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;br/&gt;&lt;center&gt;&lt;b&gt;Local&lt;/center&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>photo</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;i&gt;Para reporte de sismos ou réplicas e de danos associados&lt;/i&gt;&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;i&gt;Para reporte de danos em estruturas edificadas que possam evidenciar a ocorrência de assentamento dos solos de base (ex.: fissuras, fendilhamentos, desagregação de materiais, etc)&lt;/i&gt;&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;i&gt;Para reporte de abatimentos ou depressões nos pavimentos que possam indiciar a ocorrência de acidentes geotécnicos&lt;/i&gt;&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;i&gt;Para reporte de inundações ou acumulação indesejada de águas&lt;/i&gt;&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;i&gt;Para reporte da ocorrência de tsunamis (maremotos)&lt;/i&gt;&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>${event_type} = 'tsunami'</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;i&gt;Para reporte de outro tipo de ocorrência&lt;/i&gt;&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>${event_type} = 'other'</t>
+  </si>
+  <si>
+    <t>concat(if(${event_type} = 'earthquake', 'Sismo', if(${event_type} = 'settlement', 'Assentamento', if(${event_type} = 'landslide', 'Deslizamento', if(${event_type} = 'sinkhole', 'Abatimento', if(${event_type} = 'flood', 'Inundação', if(${event_type} = 'other', 'Outro', ${event_type})))))), " | ", format-date(${event_date}, '%Y-%m-%d'))</t>
+  </si>
+  <si>
+    <t>add_damaged_buildings_info</t>
+  </si>
+  <si>
+    <t>if(count(${floors})&gt;0, '', '&lt;br/&gt;&lt;font size=10px style="font-weight: normal"&gt;&lt;i&gt;Carregar em + para adicionar danos num ou mais edifícios&lt;/i&gt;&lt;/font&gt;')</t>
+  </si>
+  <si>
+    <t>Danos em edifícios ${add_damaged_buildings_info}</t>
+  </si>
+  <si>
+    <t>&lt;center&gt;&lt;i&gt;Para reporte de movimentos de grandes massas de solos / deslizamentos de terras e queda de muros de suporte&lt;/i&gt;&lt;/center&gt;</t>
   </si>
 </sst>
 </file>
@@ -5243,7 +5300,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5352,6 +5409,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -5366,72 +5426,6 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="22">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -5488,6 +5482,22 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -5552,6 +5562,26 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -5653,6 +5683,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <strike val="0"/>
         <condense val="0"/>
@@ -5673,6 +5723,16 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border>
@@ -5711,7 +5771,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tblSurvey" displayName="tblSurvey" ref="A1:AJ164" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tblSurvey" displayName="tblSurvey" ref="A1:AJ167" totalsRowShown="0" headerRowDxfId="19">
   <tableColumns count="36">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="type"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name"/>
@@ -5755,12 +5815,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="tblQuestionTypes" displayName="tblQuestionTypes" ref="A1:D30" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="tblQuestionTypes" displayName="tblQuestionTypes" ref="A1:D30" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Question type" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Description" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Field app" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Web app" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Question type" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Description" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Field app" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Web app" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -5769,8 +5829,8 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="tblEsriFieldTypes" displayName="tblEsriFieldTypes" ref="A1:C10" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Esri field types" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Use the bind::esri:fieldType column to control the field type created in the feature layer." dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Esri field types" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Use the bind::esri:fieldType column to control the field type created in the feature layer." dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Learn more"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5780,8 +5840,8 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="tblBindTypes" displayName="tblBindTypes" ref="A16:C22" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Bind types" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Use in the bind::type column to overwrite default field type during a survey." dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Bind types" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Use in the bind::type column to overwrite default field type during a survey." dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Learn more"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5789,12 +5849,12 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="tblReserved" displayName="tblReserved" ref="A1:A1037" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="tblReserved" displayName="tblReserved" ref="A1:A1037" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A1037">
     <sortCondition ref="A2:A1037"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Reserved keywords" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Reserved keywords" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6100,11 +6160,11 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:AJ65"/>
+  <dimension ref="A1:AJ76"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A18" sqref="A18:XFD18"/>
+      <selection pane="topRight" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6235,10 +6295,10 @@
         <v>37</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>1486</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="3" spans="1:36" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -6246,16 +6306,16 @@
         <v>37</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>1485</v>
+        <v>1482</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="F3" s="37" t="s">
         <v>110</v>
       </c>
       <c r="K3" s="37" t="s">
-        <v>1674</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="4" spans="1:36" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -6263,10 +6323,10 @@
         <v>37</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>1487</v>
+        <v>1484</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="F4" s="38" t="s">
         <v>110</v>
@@ -6278,732 +6338,918 @@
         <v>100</v>
       </c>
       <c r="B6" s="45" t="s">
-        <v>1668</v>
+        <v>1649</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>1488</v>
+        <v>1485</v>
       </c>
       <c r="F6" s="45" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:36" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+    <row r="7" spans="1:36" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="45" t="s">
-        <v>1488</v>
-      </c>
-      <c r="R7" s="45" t="s">
-        <v>1670</v>
-      </c>
-    </row>
-    <row r="8" spans="1:36" s="45" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="C7" s="49" t="s">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="46" t="s">
-        <v>1673</v>
-      </c>
-    </row>
-    <row r="9" spans="1:36" s="45" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="C8" s="48" t="s">
+        <v>1485</v>
+      </c>
+      <c r="R8" s="48" t="s">
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="46" t="s">
-        <v>1671</v>
-      </c>
-      <c r="D9" s="45" t="s">
-        <v>1672</v>
+      <c r="C9" s="45" t="s">
+        <v>1485</v>
       </c>
       <c r="R9" s="45" t="s">
-        <v>1669</v>
-      </c>
-    </row>
-    <row r="10" spans="1:36" s="45" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1651</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" s="45" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>1485</v>
+      </c>
+      <c r="R11" s="49" t="s">
+        <v>1661</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" s="45" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>1660</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>1652</v>
+      </c>
+      <c r="R12" s="45" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="45" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:36" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>1464</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>1465</v>
-      </c>
-      <c r="F12" s="32" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
-        <v>1490</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>1466</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>1488</v>
-      </c>
-      <c r="F13" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="R13" s="32" t="s">
-        <v>1529</v>
-      </c>
-    </row>
+    <row r="14" spans="1:36" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>1464</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>1667</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>1487</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>1485</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="R16" s="32" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>1684</v>
+      </c>
+      <c r="N17" s="32" t="s">
+        <v>1630</v>
+      </c>
+      <c r="T17" s="32" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>1685</v>
+      </c>
+      <c r="N18" s="32" t="s">
+        <v>1513</v>
+      </c>
+      <c r="T18" s="32" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>1696</v>
+      </c>
+      <c r="N19" s="37" t="s">
+        <v>1572</v>
+      </c>
+      <c r="T19" s="37" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>1686</v>
+      </c>
+      <c r="N20" s="37" t="s">
+        <v>1598</v>
+      </c>
+      <c r="T20" s="37" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>1687</v>
+      </c>
+      <c r="N21" s="37" t="s">
+        <v>1596</v>
+      </c>
+      <c r="T21" s="37" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="39" t="s">
+        <v>1688</v>
+      </c>
+      <c r="N22" s="39" t="s">
+        <v>1689</v>
+      </c>
+      <c r="T22" s="39" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>1690</v>
+      </c>
+      <c r="N23" s="39" t="s">
+        <v>1691</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>1485</v>
+      </c>
+      <c r="R24" s="39" t="s">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="37" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:36" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:35" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B27" s="32" t="s">
+        <v>1509</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>1510</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="N27" s="32" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C28" s="46" t="s">
+        <v>1485</v>
+      </c>
+      <c r="F28" s="40" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C29" s="46" t="s">
+        <v>1467</v>
+      </c>
+      <c r="F29" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="W29" s="40" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" s="46"/>
+    </row>
+    <row r="31" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="46"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>1478</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>1668</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="N32" s="32" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="33" spans="1:35" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" s="42" t="s">
         <v>1479</v>
       </c>
-      <c r="C17" s="37" t="s">
-        <v>1484</v>
-      </c>
-      <c r="F17" s="37" t="s">
+      <c r="C33" s="42" t="s">
+        <v>1669</v>
+      </c>
+      <c r="G33" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="H33" s="42" t="s">
+        <v>1658</v>
+      </c>
+      <c r="AH33" s="42" t="s">
+        <v>1515</v>
+      </c>
+      <c r="AI33" s="42" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="34" spans="1:35" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="42" t="s">
+        <v>1488</v>
+      </c>
+      <c r="C34" s="42" t="s">
+        <v>1671</v>
+      </c>
+      <c r="J34" s="42" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="35" spans="1:35" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="42" t="s">
+        <v>1492</v>
+      </c>
+      <c r="B35" s="42" t="s">
+        <v>1491</v>
+      </c>
+      <c r="C35" s="42" t="s">
+        <v>1485</v>
+      </c>
+      <c r="T35" s="42" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="36" spans="1:35" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="42" t="s">
+        <v>1507</v>
+      </c>
+      <c r="B36" s="42" t="s">
+        <v>1506</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="37" spans="1:35" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="42" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35" s="42" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:35" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="B39" s="42" t="s">
+        <v>1512</v>
+      </c>
+      <c r="C39" s="42" t="s">
+        <v>1485</v>
+      </c>
+      <c r="F39" s="42" t="s">
         <v>181</v>
       </c>
-      <c r="N17" s="37" t="s">
-        <v>1497</v>
-      </c>
-    </row>
-    <row r="18" spans="1:35" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" s="37" t="s">
-        <v>1480</v>
-      </c>
-      <c r="C18" s="37" t="s">
-        <v>1481</v>
-      </c>
-      <c r="AH18" s="37" t="s">
-        <v>1522</v>
-      </c>
-      <c r="AI18" s="37" t="s">
-        <v>1523</v>
-      </c>
-    </row>
-    <row r="19" spans="1:35" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="39" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" s="39" t="s">
-        <v>1491</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>1492</v>
-      </c>
-      <c r="J19" s="39" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="20" spans="1:35" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
-        <v>1496</v>
-      </c>
-      <c r="B20" s="39" t="s">
-        <v>1495</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>1488</v>
-      </c>
-      <c r="T20" s="39" t="s">
+      <c r="N39" s="42" t="s">
+        <v>1513</v>
+      </c>
+      <c r="P39" s="42">
+        <v>1</v>
+      </c>
+      <c r="X39" s="42" t="s">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="40" spans="1:35" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="42" t="s">
+        <v>1519</v>
+      </c>
+      <c r="B40" s="42" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C40" s="42" t="s">
+        <v>1675</v>
+      </c>
+      <c r="F40" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="R40" s="42" t="s">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="41" spans="1:35" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="43" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B41" s="43" t="s">
+        <v>1528</v>
+      </c>
+      <c r="C41" s="43" t="s">
+        <v>1676</v>
+      </c>
+      <c r="F41" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="R41" s="43" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="42" spans="1:35" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="43" t="s">
+        <v>1543</v>
+      </c>
+      <c r="B42" s="43" t="s">
+        <v>1530</v>
+      </c>
+      <c r="C42" s="43" t="s">
+        <v>1677</v>
+      </c>
+      <c r="F42" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="R42" s="43" t="s">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="43" spans="1:35" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="43" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B43" s="43" t="s">
+        <v>1545</v>
+      </c>
+      <c r="C43" s="43" t="s">
+        <v>1678</v>
+      </c>
+      <c r="F43" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="T43" s="43" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="21" spans="1:35" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
-        <v>1511</v>
-      </c>
-      <c r="B21" s="39" t="s">
-        <v>1510</v>
-      </c>
-      <c r="C21" s="39" t="s">
-        <v>1512</v>
-      </c>
-    </row>
-    <row r="22" spans="1:35" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="37" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+    <row r="44" spans="1:35" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="42" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="B24" s="32" t="s">
-        <v>1519</v>
-      </c>
-      <c r="C24" s="32" t="s">
-        <v>1488</v>
-      </c>
-      <c r="F24" s="32" t="s">
+      <c r="B46" s="44" t="s">
+        <v>1553</v>
+      </c>
+      <c r="C46" s="44" t="s">
+        <v>1485</v>
+      </c>
+      <c r="F46" s="44" t="s">
         <v>181</v>
       </c>
-      <c r="N24" s="32" t="s">
-        <v>1520</v>
-      </c>
-      <c r="P24" s="32">
+      <c r="N46" s="44" t="s">
+        <v>1572</v>
+      </c>
+      <c r="P46" s="44">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:35" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="40" t="s">
-        <v>1526</v>
-      </c>
-      <c r="B25" s="40" t="s">
-        <v>1524</v>
-      </c>
-      <c r="C25" s="40" t="s">
-        <v>1527</v>
-      </c>
-      <c r="F25" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="R25" s="40" t="s">
-        <v>1528</v>
-      </c>
-    </row>
-    <row r="26" spans="1:35" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="40" t="s">
-        <v>1535</v>
-      </c>
-      <c r="B26" s="40" t="s">
-        <v>1536</v>
-      </c>
-      <c r="C26" s="40" t="s">
-        <v>1537</v>
-      </c>
-      <c r="F26" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="R26" s="40" t="s">
-        <v>1538</v>
-      </c>
-    </row>
-    <row r="27" spans="1:35" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="41" t="s">
-        <v>1553</v>
-      </c>
-      <c r="B27" s="41" t="s">
-        <v>1539</v>
-      </c>
-      <c r="C27" s="41" t="s">
-        <v>1540</v>
-      </c>
-      <c r="F27" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="R27" s="41" t="s">
+      <c r="X46" s="44" t="s">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="47" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="44" t="s">
+        <v>1573</v>
+      </c>
+      <c r="B47" s="44" t="s">
         <v>1554</v>
       </c>
-    </row>
-    <row r="28" spans="1:35" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="42" t="s">
-        <v>1557</v>
-      </c>
-      <c r="B28" s="42" t="s">
-        <v>1555</v>
-      </c>
-      <c r="C28" s="42" t="s">
-        <v>1556</v>
-      </c>
-      <c r="F28" s="42" t="s">
-        <v>141</v>
-      </c>
-      <c r="T28" s="42" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="30" spans="1:35" s="42" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:35" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="B31" s="42" t="s">
-        <v>1564</v>
-      </c>
-      <c r="C31" s="42" t="s">
-        <v>1488</v>
-      </c>
-      <c r="F31" s="42" t="s">
-        <v>181</v>
-      </c>
-      <c r="N31" s="42" t="s">
-        <v>1584</v>
-      </c>
-      <c r="P31" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:35" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="42" t="s">
-        <v>1585</v>
-      </c>
-      <c r="B32" s="42" t="s">
-        <v>1565</v>
-      </c>
-      <c r="C32" s="42" t="s">
-        <v>1566</v>
-      </c>
-      <c r="F32" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="R32" s="42" t="s">
-        <v>1583</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="42" t="s">
-        <v>1567</v>
-      </c>
-      <c r="C33" s="42" t="s">
-        <v>1568</v>
-      </c>
-      <c r="F33" s="42" t="s">
-        <v>143</v>
-      </c>
-      <c r="N33" s="42" t="s">
-        <v>1570</v>
-      </c>
-      <c r="W33" s="42" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="42" t="s">
-        <v>1589</v>
-      </c>
-      <c r="B34" s="42" t="s">
-        <v>1587</v>
-      </c>
-      <c r="C34" s="42" t="s">
-        <v>1588</v>
-      </c>
-      <c r="D34" s="42" t="s">
-        <v>1675</v>
-      </c>
-      <c r="F34" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="R34" s="42" t="s">
-        <v>1596</v>
-      </c>
-      <c r="T34" s="42" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="42" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="36" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="B37" s="42" t="s">
-        <v>1597</v>
-      </c>
-      <c r="C37" s="42" t="s">
-        <v>1488</v>
-      </c>
-      <c r="F37" s="42" t="s">
-        <v>181</v>
-      </c>
-      <c r="N37" s="42" t="s">
-        <v>1610</v>
-      </c>
-      <c r="P37" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:23" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="43" t="s">
-        <v>1601</v>
-      </c>
-      <c r="B38" s="43" t="s">
-        <v>1598</v>
-      </c>
-      <c r="C38" s="43" t="s">
-        <v>1566</v>
-      </c>
-      <c r="F38" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="R38" s="43" t="s">
-        <v>1605</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="B39" s="43" t="s">
-        <v>1599</v>
-      </c>
-      <c r="C39" s="43" t="s">
-        <v>1568</v>
-      </c>
-      <c r="F39" s="43" t="s">
-        <v>143</v>
-      </c>
-      <c r="N39" s="43" t="s">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="40" spans="1:23" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="43" t="s">
-        <v>1609</v>
-      </c>
-      <c r="B40" s="43" t="s">
-        <v>1606</v>
-      </c>
-      <c r="C40" s="43" t="s">
-        <v>1607</v>
-      </c>
-      <c r="F40" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="R40" s="43" t="s">
-        <v>1608</v>
-      </c>
-      <c r="T40" s="43" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="41" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="42" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="43" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="B43" s="44" t="s">
-        <v>1611</v>
-      </c>
-      <c r="C43" s="44" t="s">
-        <v>1488</v>
-      </c>
-      <c r="F43" s="44" t="s">
-        <v>181</v>
-      </c>
-      <c r="N43" s="44" t="s">
-        <v>1612</v>
-      </c>
-      <c r="P43" s="44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="44" t="s">
-        <v>1614</v>
-      </c>
-      <c r="B44" s="44" t="s">
-        <v>1613</v>
-      </c>
-      <c r="C44" s="44" t="s">
-        <v>1617</v>
-      </c>
-      <c r="F44" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="T44" s="44" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="45" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="44" t="s">
-        <v>1620</v>
-      </c>
-      <c r="B45" s="44" t="s">
-        <v>1618</v>
-      </c>
-      <c r="C45" s="44" t="s">
-        <v>1619</v>
-      </c>
-      <c r="F45" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="R45" s="44" t="s">
-        <v>1624</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="B46" s="44" t="s">
-        <v>1622</v>
-      </c>
-      <c r="C46" s="44" t="s">
-        <v>1623</v>
-      </c>
-      <c r="F46" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="N46" s="44" t="s">
-        <v>1621</v>
-      </c>
-    </row>
-    <row r="47" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="44" t="s">
-        <v>1631</v>
-      </c>
-      <c r="B47" s="44" t="s">
-        <v>1633</v>
-      </c>
       <c r="C47" s="44" t="s">
-        <v>1629</v>
+        <v>1672</v>
       </c>
       <c r="F47" s="44" t="s">
         <v>36</v>
       </c>
       <c r="R47" s="44" t="s">
-        <v>1630</v>
-      </c>
-    </row>
-    <row r="48" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="48" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="44" t="s">
         <v>63</v>
       </c>
       <c r="B48" s="44" t="s">
-        <v>1634</v>
+        <v>1555</v>
       </c>
       <c r="C48" s="44" t="s">
-        <v>1582</v>
+        <v>1556</v>
       </c>
       <c r="F48" s="44" t="s">
         <v>143</v>
       </c>
       <c r="N48" s="44" t="s">
+        <v>1558</v>
+      </c>
+      <c r="W48" s="44" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="44" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B49" s="44" t="s">
+        <v>1575</v>
+      </c>
+      <c r="C49" s="44" t="s">
+        <v>1673</v>
+      </c>
+      <c r="D49" s="44" t="s">
+        <v>1674</v>
+      </c>
+      <c r="F49" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="R49" s="44" t="s">
+        <v>1583</v>
+      </c>
+      <c r="T49" s="44" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="B52" s="44" t="s">
+        <v>1584</v>
+      </c>
+      <c r="C52" s="44" t="s">
+        <v>1485</v>
+      </c>
+      <c r="F52" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="N52" s="44" t="s">
+        <v>1596</v>
+      </c>
+      <c r="P52" s="44">
+        <v>1</v>
+      </c>
+      <c r="X52" s="44" t="s">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="44" t="s">
+        <v>1588</v>
+      </c>
+      <c r="B53" s="44" t="s">
+        <v>1585</v>
+      </c>
+      <c r="C53" s="44" t="s">
+        <v>1672</v>
+      </c>
+      <c r="F53" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="R53" s="44" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" s="44" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C54" s="44" t="s">
+        <v>1556</v>
+      </c>
+      <c r="F54" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="N54" s="44" t="s">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="44" t="s">
+        <v>1595</v>
+      </c>
+      <c r="B55" s="44" t="s">
+        <v>1593</v>
+      </c>
+      <c r="C55" s="44" t="s">
+        <v>1679</v>
+      </c>
+      <c r="F55" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="R55" s="44" t="s">
+        <v>1594</v>
+      </c>
+      <c r="T55" s="44" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:24" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" s="43" t="s">
+        <v>1597</v>
+      </c>
+      <c r="C58" s="43" t="s">
+        <v>1485</v>
+      </c>
+      <c r="F58" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="N58" s="43" t="s">
+        <v>1598</v>
+      </c>
+      <c r="P58" s="43">
+        <v>1</v>
+      </c>
+      <c r="X58" s="43" t="s">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A59" s="32" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B59" s="32" t="s">
+        <v>1599</v>
+      </c>
+      <c r="C59" s="32" t="s">
+        <v>1680</v>
+      </c>
+      <c r="F59" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="N59" s="39"/>
+      <c r="T59" s="32" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="39" t="s">
+        <v>1604</v>
+      </c>
+      <c r="B60" s="39" t="s">
+        <v>1603</v>
+      </c>
+      <c r="C60" s="39" t="s">
+        <v>1682</v>
+      </c>
+      <c r="F60" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="R60" s="39" t="s">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" s="39" t="s">
+        <v>1606</v>
+      </c>
+      <c r="C61" s="39" t="s">
+        <v>1607</v>
+      </c>
+      <c r="F61" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="N61" s="39" t="s">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A62" s="32" t="s">
+        <v>1614</v>
+      </c>
+      <c r="B62" s="32" t="s">
+        <v>1616</v>
+      </c>
+      <c r="C62" s="32" t="s">
+        <v>1681</v>
+      </c>
+      <c r="F62" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="R62" s="32" t="s">
+        <v>1613</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="44" t="s">
+        <v>1617</v>
+      </c>
+      <c r="C63" s="44" t="s">
+        <v>1570</v>
+      </c>
+      <c r="F63" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="N63" s="44" t="s">
+        <v>1615</v>
+      </c>
+      <c r="W63" s="44" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="65" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:24" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="B66" s="50" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C66" s="50" t="s">
+        <v>1485</v>
+      </c>
+      <c r="F66" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="K66" s="50" t="s">
+        <v>1694</v>
+      </c>
+      <c r="T66" s="50" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="67" spans="1:24" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="B67" s="50" t="s">
+        <v>1631</v>
+      </c>
+      <c r="C67" s="50" t="s">
+        <v>1695</v>
+      </c>
+      <c r="F67" s="50" t="s">
+        <v>181</v>
+      </c>
+      <c r="N67" s="50" t="s">
+        <v>1630</v>
+      </c>
+      <c r="X67" s="50" t="s">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="68" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="44" t="s">
+        <v>1634</v>
+      </c>
+      <c r="B68" s="44" t="s">
+        <v>1635</v>
+      </c>
+      <c r="C68" s="44" t="s">
+        <v>1485</v>
+      </c>
+      <c r="F68" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="G68" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="R68" s="44" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A69" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B69" s="32" t="s">
         <v>1632</v>
       </c>
-      <c r="W48" s="44" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="49" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="44" t="s">
+      <c r="C69" s="32" t="s">
+        <v>1633</v>
+      </c>
+      <c r="F69" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="J69" s="32">
+        <v>1</v>
+      </c>
+      <c r="T69" s="32" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A70" s="32" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="B51" s="44" t="s">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A72" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B72" s="32" t="s">
+        <v>1629</v>
+      </c>
+      <c r="C72" s="32" t="s">
+        <v>1485</v>
+      </c>
+      <c r="F72" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="N72" s="32" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A73" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C73" s="32" t="s">
+        <v>1665</v>
+      </c>
+      <c r="W73" s="32" t="s">
         <v>1648</v>
       </c>
-      <c r="C51" s="44" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F51" s="44" t="s">
-        <v>181</v>
-      </c>
-      <c r="N51" s="44" t="s">
-        <v>1647</v>
-      </c>
-    </row>
-    <row r="52" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="44" t="s">
-        <v>1651</v>
-      </c>
-      <c r="B52" s="44" t="s">
-        <v>1653</v>
-      </c>
-      <c r="C52" s="44" t="s">
-        <v>1488</v>
-      </c>
-      <c r="F52" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="G52" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="R52" s="44" t="s">
-        <v>1663</v>
-      </c>
-    </row>
-    <row r="53" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="B53" s="44" t="s">
-        <v>1649</v>
-      </c>
-      <c r="C53" s="44" t="s">
-        <v>1650</v>
-      </c>
-      <c r="F53" s="44" t="s">
-        <v>158</v>
-      </c>
-      <c r="J53" s="44">
-        <v>1</v>
-      </c>
-      <c r="T53" s="44" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="54" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="44" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="1:23" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A56" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B56" s="32" t="s">
-        <v>1514</v>
-      </c>
-      <c r="C56" s="32" t="s">
-        <v>1516</v>
-      </c>
-      <c r="F56" s="32" t="s">
-        <v>181</v>
-      </c>
-      <c r="N56" s="39" t="s">
-        <v>1497</v>
-      </c>
-    </row>
-    <row r="57" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="B57" s="39" t="s">
-        <v>1517</v>
-      </c>
-      <c r="C57" s="39" t="s">
-        <v>1488</v>
-      </c>
-    </row>
-    <row r="58" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="B58" s="39" t="s">
-        <v>1515</v>
-      </c>
-      <c r="C58" s="39" t="s">
-        <v>1516</v>
-      </c>
-    </row>
-    <row r="59" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="39" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="60" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="B60" s="39" t="s">
-        <v>1467</v>
-      </c>
-      <c r="C60" s="39" t="s">
-        <v>1468</v>
-      </c>
-      <c r="F60" s="39" t="s">
-        <v>143</v>
-      </c>
-      <c r="W60" s="39" t="s">
-        <v>1518</v>
-      </c>
-    </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A61" s="32" t="s">
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A74" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C74" s="32" t="s">
+        <v>1485</v>
+      </c>
+      <c r="R74" s="32" t="s">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A75" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C75" s="32" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A76" s="32" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="62" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="B63" s="44" t="s">
-        <v>1646</v>
-      </c>
-      <c r="C63" s="44" t="s">
-        <v>1488</v>
-      </c>
-      <c r="F63" s="44" t="s">
-        <v>181</v>
-      </c>
-      <c r="N63" s="44" t="s">
-        <v>1647</v>
-      </c>
-    </row>
-    <row r="64" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="C64" s="44" t="s">
-        <v>1667</v>
-      </c>
-      <c r="W64" s="44" t="s">
-        <v>1666</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="44" t="s">
-        <v>102</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B164">
-    <cfRule type="duplicateValues" dxfId="6" priority="15"/>
+  <conditionalFormatting sqref="B2:B167">
+    <cfRule type="duplicateValues" dxfId="20" priority="19"/>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" sqref="A2:A164" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="A2:A167" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>QuestionTypes</formula1>
     </dataValidation>
-    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Name" error="Names must be unique and cannot contain spaces, non-ASCII characters, reserved keywords, or special symbols. For ArcGIS Enterprise feature layers, names must not exceed 31 characters." sqref="B2:B164" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Name" error="Names must be unique and cannot contain spaces, non-ASCII characters, reserved keywords, or special symbols. For ArcGIS Enterprise feature layers, names must not exceed 31 characters." sqref="B2:B167" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>AND(LEN(B2)=LEN(SUBSTITUTE(B2," ","")),LEN(B2)&lt;32,COUNTIF(Reserved,B2) = 0,SUMPRODUCT(--ISNUMBER(SEARCH(SpecialChars,B2)))=0)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="I2:I164 G2:G164" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" sqref="I2:I167 G2:G167" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Bind Type" error="The value you have entered is not one of the supported bind types." sqref="S2:S164" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Bind Type" error="The value you have entered is not one of the supported bind types." sqref="S2:S167" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>BindTypes</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Field Type" error="The value you have entered is not one of the supported field types." sqref="T2:T164" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Field Type" error="The value you have entered is not one of the supported field types." sqref="T2:T167" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>EsriFieldTypes</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Field Length" error="Please enter a whole number greater than zero." sqref="U2:U164" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Field Length" error="Please enter a whole number greater than zero." sqref="U2:U167" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F164" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F167" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>IF(LEFT(A2,4)="rank",appearRank,IF(LEFT(A2,8)="select_m",appearSelMulti,IF(LEFT(A2,8)="select_o",appearSelOne,IF(A2="begin group",appearBeginGrp,IF(A2="begin repeat",appearBeginRpt,INDIRECT("appear"&amp;A2))))))</formula1>
     </dataValidation>
   </dataValidations>
@@ -7022,8 +7268,8 @@
   </sheetPr>
   <dimension ref="A1:F224"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7060,24 +7306,24 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>1470</v>
+      </c>
+      <c r="B4" t="s">
         <v>1471</v>
       </c>
-      <c r="B4" t="s">
-        <v>1472</v>
-      </c>
       <c r="C4" t="s">
-        <v>1665</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -7087,854 +7333,860 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1489</v>
+        <v>1486</v>
       </c>
       <c r="B6" t="s">
-        <v>1498</v>
+        <v>1494</v>
       </c>
       <c r="C6" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
-        <v>1489</v>
+        <v>1486</v>
       </c>
       <c r="B7" t="s">
-        <v>1499</v>
+        <v>1495</v>
       </c>
       <c r="C7" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
-        <v>1489</v>
+        <v>1486</v>
       </c>
       <c r="B8" t="s">
-        <v>1500</v>
+        <v>1496</v>
       </c>
       <c r="C8" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
-        <v>1489</v>
+        <v>1486</v>
       </c>
       <c r="B9" t="s">
-        <v>1502</v>
+        <v>1498</v>
       </c>
       <c r="C9" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="39" t="s">
-        <v>1489</v>
+        <v>1486</v>
       </c>
       <c r="B10" t="s">
-        <v>1501</v>
+        <v>1497</v>
       </c>
       <c r="C10" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="39" t="s">
-        <v>1489</v>
+        <v>1486</v>
       </c>
       <c r="B11" t="s">
-        <v>1513</v>
+        <v>1508</v>
       </c>
       <c r="C11" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="47" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>1654</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>1655</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1564</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>1489</v>
       </c>
-      <c r="B12" s="47" t="s">
-        <v>1676</v>
-      </c>
-      <c r="C12" s="47" t="s">
-        <v>1677</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>1493</v>
-      </c>
-      <c r="B14">
+      <c r="B15">
         <v>1</v>
       </c>
-      <c r="C14" t="s">
-        <v>1494</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
+      <c r="C15" t="s">
+        <v>1490</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>1503</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1504</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1507</v>
-      </c>
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="39" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1500</v>
+      </c>
+      <c r="C17" t="s">
         <v>1503</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1505</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1508</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="39" t="s">
-        <v>1503</v>
+        <v>1499</v>
       </c>
       <c r="B18" t="s">
-        <v>1506</v>
+        <v>1501</v>
       </c>
       <c r="C18" t="s">
-        <v>1509</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
+      <c r="A19" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1502</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1505</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>1525</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="s">
-        <v>1525</v>
+        <v>1518</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="s">
-        <v>1525</v>
+        <v>1518</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="40" t="s">
-        <v>1525</v>
+        <v>1518</v>
       </c>
       <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="32" t="s">
+        <v>1518</v>
+      </c>
+      <c r="B24" s="32">
         <v>4</v>
       </c>
-      <c r="C23">
+      <c r="C24" s="32">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>1530</v>
-      </c>
-      <c r="B25" t="s">
-        <v>1531</v>
-      </c>
-      <c r="C25" t="s">
-        <v>1532</v>
-      </c>
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="s">
-        <v>1530</v>
+        <v>1522</v>
       </c>
       <c r="B26" t="s">
-        <v>1533</v>
+        <v>1523</v>
       </c>
       <c r="C26" t="s">
-        <v>1534</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27"/>
-      <c r="B27"/>
-      <c r="C27"/>
+      <c r="A27" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1526</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>1541</v>
-      </c>
-      <c r="B28" t="s">
-        <v>1542</v>
-      </c>
-      <c r="C28" t="s">
-        <v>1543</v>
-      </c>
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="41" t="s">
-        <v>1541</v>
+        <v>1531</v>
       </c>
       <c r="B29" t="s">
-        <v>132</v>
+        <v>1532</v>
       </c>
       <c r="C29" t="s">
-        <v>1544</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="41" t="s">
-        <v>1541</v>
+        <v>1531</v>
       </c>
       <c r="B30" t="s">
-        <v>1545</v>
+        <v>132</v>
       </c>
       <c r="C30" t="s">
-        <v>1546</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="41" t="s">
-        <v>1541</v>
+        <v>1531</v>
       </c>
       <c r="B31" t="s">
-        <v>1547</v>
+        <v>1535</v>
       </c>
       <c r="C31" t="s">
-        <v>1548</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="41" t="s">
-        <v>1541</v>
+        <v>1531</v>
       </c>
       <c r="B32" t="s">
-        <v>1549</v>
+        <v>1537</v>
       </c>
       <c r="C32" t="s">
-        <v>1550</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1539</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B34" t="s">
         <v>1541</v>
       </c>
-      <c r="B33" t="s">
-        <v>1551</v>
-      </c>
-      <c r="C33" t="s">
-        <v>1552</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34"/>
+      <c r="C34" t="s">
+        <v>1542</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>1558</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
-        <v>1560</v>
-      </c>
+      <c r="A35"/>
+      <c r="B35"/>
+      <c r="C35"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
-        <v>1558</v>
+        <v>1547</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>1559</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="42" t="s">
-        <v>1558</v>
+        <v>1547</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>1561</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="42" t="s">
-        <v>1558</v>
+        <v>1547</v>
       </c>
       <c r="B38">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>1562</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="42" t="s">
-        <v>1558</v>
+        <v>1547</v>
       </c>
       <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="42" t="s">
+        <v>1547</v>
+      </c>
+      <c r="B40">
         <v>5</v>
       </c>
-      <c r="C39" t="s">
-        <v>1563</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="42"/>
-      <c r="B40"/>
-      <c r="C40"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="32" t="s">
-        <v>1586</v>
-      </c>
-      <c r="B41" s="32" t="s">
-        <v>1571</v>
-      </c>
-      <c r="C41" s="32" t="s">
-        <v>1577</v>
+      <c r="C40" t="s">
+        <v>1552</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="42" t="s">
-        <v>1586</v>
+        <v>1574</v>
       </c>
       <c r="B42" t="s">
-        <v>1572</v>
+        <v>1559</v>
       </c>
       <c r="C42" t="s">
-        <v>1578</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="42" t="s">
-        <v>1586</v>
+        <v>1574</v>
       </c>
       <c r="B43" t="s">
-        <v>1573</v>
+        <v>1560</v>
       </c>
       <c r="C43" t="s">
-        <v>1579</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="42" t="s">
-        <v>1586</v>
+        <v>1574</v>
       </c>
       <c r="B44" t="s">
-        <v>1574</v>
+        <v>1561</v>
       </c>
       <c r="C44" t="s">
-        <v>1580</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="42" t="s">
-        <v>1586</v>
+        <v>1574</v>
       </c>
       <c r="B45" t="s">
-        <v>1575</v>
+        <v>1562</v>
       </c>
       <c r="C45" t="s">
-        <v>1581</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="42" t="s">
-        <v>1586</v>
+        <v>1574</v>
       </c>
       <c r="B46" t="s">
-        <v>1576</v>
+        <v>1563</v>
       </c>
       <c r="C46" t="s">
-        <v>1582</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47"/>
-      <c r="B47"/>
-      <c r="C47"/>
+      <c r="A47" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1564</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1570</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>1590</v>
-      </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48" t="s">
-        <v>1591</v>
-      </c>
+      <c r="A48"/>
+      <c r="B48"/>
+      <c r="C48"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="42" t="s">
-        <v>1590</v>
+        <v>1577</v>
       </c>
       <c r="B49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>1592</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="42" t="s">
-        <v>1590</v>
+        <v>1577</v>
       </c>
       <c r="B50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>1593</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="42" t="s">
-        <v>1590</v>
+        <v>1577</v>
       </c>
       <c r="B51" s="32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>1595</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="42" t="s">
-        <v>1590</v>
+        <v>1577</v>
       </c>
       <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>1577</v>
+      </c>
+      <c r="B53">
         <v>5</v>
       </c>
-      <c r="C52" t="s">
-        <v>1594</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53"/>
-      <c r="B53"/>
-      <c r="C53"/>
+      <c r="C53" t="s">
+        <v>1581</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>1602</v>
-      </c>
-      <c r="B54" s="43" t="s">
-        <v>1571</v>
-      </c>
-      <c r="C54" s="43" t="s">
-        <v>1577</v>
-      </c>
+      <c r="A54"/>
+      <c r="B54" s="43"/>
+      <c r="C54" s="43"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="43" t="s">
-        <v>1602</v>
+        <v>1589</v>
       </c>
       <c r="B55" s="43" t="s">
-        <v>1572</v>
+        <v>1559</v>
       </c>
       <c r="C55" s="43" t="s">
-        <v>1578</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="43" t="s">
-        <v>1602</v>
+        <v>1589</v>
       </c>
       <c r="B56" s="43" t="s">
-        <v>1573</v>
+        <v>1560</v>
       </c>
       <c r="C56" s="43" t="s">
-        <v>1579</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="43" t="s">
-        <v>1602</v>
+        <v>1589</v>
       </c>
       <c r="B57" s="43" t="s">
-        <v>1574</v>
+        <v>1561</v>
       </c>
       <c r="C57" s="43" t="s">
-        <v>1580</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="43" t="s">
-        <v>1602</v>
+        <v>1589</v>
       </c>
       <c r="B58" s="43" t="s">
-        <v>1604</v>
+        <v>1562</v>
       </c>
       <c r="C58" s="43" t="s">
-        <v>1603</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="43" t="s">
-        <v>1602</v>
+        <v>1589</v>
       </c>
       <c r="B59" s="43" t="s">
-        <v>1576</v>
+        <v>1591</v>
       </c>
       <c r="C59" s="43" t="s">
-        <v>1582</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60"/>
-      <c r="B60"/>
-      <c r="C60"/>
+      <c r="A60" t="s">
+        <v>1589</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1564</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1570</v>
+      </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>1606</v>
-      </c>
-      <c r="B61">
-        <v>1</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
-      </c>
+      <c r="A61"/>
+      <c r="B61"/>
+      <c r="C61"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="43" t="s">
-        <v>1606</v>
+        <v>1593</v>
       </c>
       <c r="B62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C62">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="43" t="s">
-        <v>1606</v>
+        <v>1593</v>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C63">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="43" t="s">
-        <v>1606</v>
+        <v>1593</v>
       </c>
       <c r="B64" s="32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C64" s="32">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="43" t="s">
-        <v>1606</v>
+        <v>1593</v>
       </c>
       <c r="B65">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C65">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="43" t="s">
-        <v>1606</v>
+        <v>1593</v>
       </c>
       <c r="B66">
+        <v>5</v>
+      </c>
+      <c r="C66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>1593</v>
+      </c>
+      <c r="B67">
         <v>6</v>
       </c>
-      <c r="C66">
+      <c r="C67">
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67"/>
-      <c r="B67"/>
-      <c r="C67"/>
-    </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>1615</v>
-      </c>
-      <c r="B68">
-        <v>1</v>
-      </c>
-      <c r="C68">
-        <v>1</v>
-      </c>
+      <c r="A68"/>
+      <c r="B68"/>
+      <c r="C68"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="44" t="s">
-        <v>1615</v>
+        <v>1601</v>
       </c>
       <c r="B69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C69">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="44" t="s">
-        <v>1615</v>
+        <v>1601</v>
       </c>
       <c r="B70">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C70">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="44" t="s">
-        <v>1615</v>
+        <v>1601</v>
       </c>
       <c r="B71">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C71">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="44" t="s">
-        <v>1615</v>
+        <v>1601</v>
       </c>
       <c r="B72">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C72">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="44" t="s">
-        <v>1615</v>
+        <v>1601</v>
       </c>
       <c r="B73">
+        <v>5</v>
+      </c>
+      <c r="C73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>1601</v>
+      </c>
+      <c r="B74">
         <v>6</v>
       </c>
-      <c r="C73" t="s">
-        <v>1616</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74"/>
-      <c r="B74"/>
-      <c r="C74"/>
+      <c r="C74" t="s">
+        <v>1602</v>
+      </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>1625</v>
-      </c>
-      <c r="B75" t="s">
-        <v>1573</v>
-      </c>
-      <c r="C75" t="s">
-        <v>1627</v>
-      </c>
+      <c r="A75"/>
+      <c r="B75"/>
+      <c r="C75"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="44" t="s">
-        <v>1625</v>
+        <v>1609</v>
       </c>
       <c r="B76" t="s">
-        <v>1626</v>
+        <v>1561</v>
       </c>
       <c r="C76" t="s">
-        <v>1628</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="44" t="s">
-        <v>1625</v>
+        <v>1609</v>
       </c>
       <c r="B77" t="s">
-        <v>1572</v>
+        <v>1610</v>
       </c>
       <c r="C77" t="s">
-        <v>1578</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="44" t="s">
-        <v>1625</v>
+        <v>1609</v>
       </c>
       <c r="B78" t="s">
-        <v>1576</v>
+        <v>1560</v>
       </c>
       <c r="C78" t="s">
-        <v>1623</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="44"/>
-      <c r="B79"/>
-      <c r="C79"/>
+      <c r="A79" s="44" t="s">
+        <v>1609</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1564</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1607</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="44" t="s">
-        <v>1635</v>
-      </c>
-      <c r="B80" t="s">
-        <v>1636</v>
-      </c>
-      <c r="C80" t="s">
-        <v>1641</v>
-      </c>
+      <c r="A80" s="44"/>
+      <c r="B80"/>
+      <c r="C80"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="44" t="s">
-        <v>1635</v>
+        <v>1618</v>
       </c>
       <c r="B81" t="s">
-        <v>1637</v>
+        <v>1619</v>
       </c>
       <c r="C81" t="s">
-        <v>1642</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="44" t="s">
-        <v>1635</v>
+        <v>1618</v>
       </c>
       <c r="B82" t="s">
-        <v>1638</v>
+        <v>1620</v>
       </c>
       <c r="C82" t="s">
-        <v>1643</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="44" t="s">
-        <v>1635</v>
+        <v>1618</v>
       </c>
       <c r="B83" t="s">
-        <v>1639</v>
+        <v>1621</v>
       </c>
       <c r="C83" t="s">
-        <v>1644</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="44" t="s">
-        <v>1635</v>
+        <v>1618</v>
       </c>
       <c r="B84" t="s">
-        <v>1640</v>
+        <v>1622</v>
       </c>
       <c r="C84" t="s">
-        <v>1645</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="44" t="s">
-        <v>1635</v>
+        <v>1618</v>
       </c>
       <c r="B85" t="s">
-        <v>1576</v>
+        <v>1623</v>
       </c>
       <c r="C85" t="s">
-        <v>1582</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86"/>
-      <c r="B86"/>
-      <c r="C86"/>
+      <c r="A86" t="s">
+        <v>1618</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1564</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1570</v>
+      </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>1654</v>
-      </c>
-      <c r="B87" t="s">
-        <v>1655</v>
-      </c>
-      <c r="C87" t="s">
-        <v>1656</v>
-      </c>
+      <c r="A87"/>
+      <c r="B87"/>
+      <c r="C87"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="44" t="s">
-        <v>1654</v>
+        <v>1636</v>
       </c>
       <c r="B88" t="s">
-        <v>1657</v>
+        <v>1637</v>
       </c>
       <c r="C88" t="s">
-        <v>1660</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="44" t="s">
-        <v>1654</v>
+        <v>1636</v>
       </c>
       <c r="B89" t="s">
-        <v>1658</v>
+        <v>1639</v>
       </c>
       <c r="C89" t="s">
-        <v>1661</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="44" t="s">
-        <v>1654</v>
+        <v>1636</v>
       </c>
       <c r="B90" t="s">
-        <v>1659</v>
+        <v>1640</v>
       </c>
       <c r="C90" t="s">
-        <v>1662</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91"/>
-      <c r="B91"/>
-      <c r="C91"/>
+      <c r="A91" t="s">
+        <v>1636</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1641</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1644</v>
+      </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92"/>
@@ -8590,7 +8842,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8632,13 +8884,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1468</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>1514</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>1692</v>
+      </c>
+      <c r="F2" s="32">
+        <v>20220907</v>
+      </c>
+      <c r="G2" s="32" t="s">
         <v>1469</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>1521</v>
-      </c>
-      <c r="G2" s="32" t="s">
-        <v>1470</v>
       </c>
       <c r="H2" t="s">
         <v>52</v>
@@ -8676,10 +8934,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="52"/>
       <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8704,10 +8962,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="49"/>
+      <c r="B6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -9159,10 +9417,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:D30">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9181,8 +9439,8 @@
   </sheetPr>
   <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10328,10 +10586,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:E34">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10541,8 +10799,8 @@
   </sheetPr>
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11554,10 +11812,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A27">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:A36">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C1" r:id="rId1" location="ESRI_SECTION1_8095742B322A4AB9BB01B2BB448426A3" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
@@ -11580,8 +11838,8 @@
   </sheetPr>
   <dimension ref="A1:B1037"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A997" workbookViewId="0">
+      <selection activeCell="A1008" sqref="A1008"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>